<commit_message>
- Supprimé une ligne vide.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20548 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2050/group.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2050/group.xlsx
@@ -627,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1476,45 +1476,57 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
+      <c r="A43" s="2">
+        <v>4040000046</v>
+      </c>
+      <c r="B43" s="7">
+        <v>2050000000</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4040010173</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="5">
+        <v>4040000147</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>4040000046</v>
+        <v>4040000047</v>
       </c>
       <c r="B44" s="7">
         <v>2050000000</v>
       </c>
       <c r="C44" s="3">
-        <v>4040010173</v>
+        <v>4040010176</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E44" s="5">
-        <v>4040000147</v>
+        <v>4000000560</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>4040000047</v>
+        <v>4040000048</v>
       </c>
       <c r="B45" s="7">
         <v>2050000000</v>
       </c>
       <c r="C45" s="3">
-        <v>4040010176</v>
+        <v>4040010177</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E45" s="5">
         <v>4000000560</v>
@@ -1525,53 +1537,53 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>4040000048</v>
+        <v>4040000049</v>
       </c>
       <c r="B46" s="7">
         <v>2050000000</v>
       </c>
       <c r="C46" s="3">
-        <v>4040010177</v>
+        <v>4040010178</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E46" s="5">
-        <v>4000000560</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>20</v>
+        <v>4000000662.0999999</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>4040000049</v>
+        <v>4040000052</v>
       </c>
       <c r="B47" s="7">
         <v>2050000000</v>
       </c>
       <c r="C47" s="3">
-        <v>4040010178</v>
+        <v>4040010180</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E47" s="5">
-        <v>4000000662.0999999</v>
+        <v>4000000662</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>4040000052</v>
+        <v>4040000053</v>
       </c>
       <c r="B48" s="7">
         <v>2050000000</v>
       </c>
       <c r="C48" s="3">
-        <v>4040010180</v>
+        <v>4040010181</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E48" s="5">
         <v>4000000662</v>
@@ -1582,16 +1594,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>4040000053</v>
+        <v>4040000054</v>
       </c>
       <c r="B49" s="7">
         <v>2050000000</v>
       </c>
       <c r="C49" s="3">
-        <v>4040010181</v>
+        <v>4040010182</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E49" s="5">
         <v>4000000662</v>
@@ -1602,16 +1614,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>4040000054</v>
+        <v>4040000055</v>
       </c>
       <c r="B50" s="7">
         <v>2050000000</v>
       </c>
       <c r="C50" s="3">
-        <v>4040010182</v>
+        <v>4040010184</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E50" s="5">
         <v>4000000662</v>
@@ -1622,16 +1634,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>4040000055</v>
+        <v>4040000056</v>
       </c>
       <c r="B51" s="7">
         <v>2050000000</v>
       </c>
       <c r="C51" s="3">
-        <v>4040010184</v>
+        <v>4040010185</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E51" s="5">
         <v>4000000662</v>
@@ -1642,16 +1654,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>4040000056</v>
+        <v>4040000057</v>
       </c>
       <c r="B52" s="7">
         <v>2050000000</v>
       </c>
       <c r="C52" s="3">
-        <v>4040010185</v>
+        <v>4040010186</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E52" s="5">
         <v>4000000662</v>
@@ -1662,16 +1674,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>4040000057</v>
+        <v>4040000058</v>
       </c>
       <c r="B53" s="7">
         <v>2050000000</v>
       </c>
       <c r="C53" s="3">
-        <v>4040010186</v>
+        <v>4040010188</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E53" s="5">
         <v>4000000662</v>
@@ -1682,16 +1694,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>4040000058</v>
+        <v>4040000059</v>
       </c>
       <c r="B54" s="7">
         <v>2050000000</v>
       </c>
       <c r="C54" s="3">
-        <v>4040010188</v>
+        <v>4040010189</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E54" s="5">
         <v>4000000662</v>
@@ -1702,16 +1714,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>4040000059</v>
+        <v>4040000060</v>
       </c>
       <c r="B55" s="7">
         <v>2050000000</v>
       </c>
       <c r="C55" s="3">
-        <v>4040010189</v>
+        <v>4040010190</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E55" s="5">
         <v>4000000662</v>
@@ -1722,16 +1734,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>4040000060</v>
+        <v>4040000061</v>
       </c>
       <c r="B56" s="7">
         <v>2050000000</v>
       </c>
       <c r="C56" s="3">
-        <v>4040010190</v>
+        <v>4040010191</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E56" s="5">
         <v>4000000662</v>
@@ -1742,16 +1754,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>4040000061</v>
+        <v>4040000062</v>
       </c>
       <c r="B57" s="7">
         <v>2050000000</v>
       </c>
       <c r="C57" s="3">
-        <v>4040010191</v>
+        <v>4040010192</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E57" s="5">
         <v>4000000662</v>
@@ -1762,16 +1774,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>4040000062</v>
+        <v>4040000063</v>
       </c>
       <c r="B58" s="7">
         <v>2050000000</v>
       </c>
       <c r="C58" s="3">
-        <v>4040010192</v>
+        <v>4040010193</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E58" s="5">
         <v>4000000662</v>
@@ -1782,16 +1794,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>4040000063</v>
+        <v>4040000064</v>
       </c>
       <c r="B59" s="7">
         <v>2050000000</v>
       </c>
       <c r="C59" s="3">
-        <v>4040010193</v>
+        <v>4040010194</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E59" s="5">
         <v>4000000662</v>
@@ -1802,16 +1814,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>4040000064</v>
+        <v>4040000066</v>
       </c>
       <c r="B60" s="7">
         <v>2050000000</v>
       </c>
       <c r="C60" s="3">
-        <v>4040010194</v>
+        <v>4040010195</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E60" s="5">
         <v>4000000662</v>
@@ -1822,16 +1834,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>4040000066</v>
+        <v>4040000065</v>
       </c>
       <c r="B61" s="7">
         <v>2050000000</v>
       </c>
       <c r="C61" s="3">
-        <v>4040010195</v>
+        <v>4040010196</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E61" s="5">
         <v>4000000662</v>
@@ -1842,16 +1854,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>4040000065</v>
+        <v>4040000067</v>
       </c>
       <c r="B62" s="7">
         <v>2050000000</v>
       </c>
       <c r="C62" s="3">
-        <v>4040010196</v>
+        <v>4040010248</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E62" s="5">
         <v>4000000662</v>
@@ -1862,16 +1874,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>4040000067</v>
+        <v>4040000068</v>
       </c>
       <c r="B63" s="7">
         <v>2050000000</v>
       </c>
       <c r="C63" s="3">
-        <v>4040010248</v>
+        <v>4040010249</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E63" s="5">
         <v>4000000662</v>
@@ -1882,16 +1894,16 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>4040000068</v>
+        <v>4040000069</v>
       </c>
       <c r="B64" s="7">
         <v>2050000000</v>
       </c>
       <c r="C64" s="3">
-        <v>4040010249</v>
+        <v>4040010250</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E64" s="5">
         <v>4000000662</v>
@@ -1901,39 +1913,19 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
-        <v>4040000069</v>
-      </c>
-      <c r="B65" s="7">
-        <v>2050000000</v>
-      </c>
-      <c r="C65" s="3">
-        <v>4040010250</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E65" s="5">
-        <v>4000000662</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>59</v>
-      </c>
+      <c r="A65" s="2"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="3"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="6"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="7"/>
       <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
       <c r="E66" s="5"/>
       <c r="F66" s="6"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>